<commit_message>
filter tube rows in multiform files
</commit_message>
<xml_diff>
--- a/api/tests/acceptance/scripts/target-profile-migrations/migration-test-multiform_1.xlsx
+++ b/api/tests/acceptance/scripts/target-profile-migrations/migration-test-multiform_1.xlsx
@@ -4,7 +4,8 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="2005" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="2006" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Feuille inutile" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="2006" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,24 +13,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+  <si>
+    <t>Parcours thématique_RGPD &amp; Données personnelles</t>
+  </si>
+  <si>
+    <t>Création : Avril 2022</t>
+  </si>
+  <si>
+    <t>1) capage</t>
+  </si>
+  <si>
+    <t>Sujet (code ou autre)</t>
+  </si>
+  <si>
+    <t>Niveau max</t>
+  </si>
+  <si>
+    <t>@codageEmblématique</t>
+  </si>
+  <si>
+    <t>@terminal</t>
+  </si>
+  <si>
+    <t>@editerDocEnLigne</t>
+  </si>
+  <si>
+    <t>@partageDroits</t>
+  </si>
+  <si>
+    <t>Coucou</t>
+  </si>
+  <si>
+    <t>les</t>
+  </si>
+  <si>
+    <t>zamiiiiiiiiiiiiis</t>
+  </si>
   <si>
     <t>id de sujet</t>
   </si>
   <si>
     <t>niveau max</t>
-  </si>
-  <si>
-    <t>@codageEmblématique</t>
-  </si>
-  <si>
-    <t>@terminal</t>
-  </si>
-  <si>
-    <t>@editerDocEnLigne</t>
-  </si>
-  <si>
-    <t>@partageDroits</t>
   </si>
   <si>
     <t>@nimp</t>
@@ -39,7 +64,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -47,17 +72,41 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <sz val="8.0"/>
       <color rgb="FF000000"/>
       <name val="&quot;Arial&quot;"/>
     </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF666666"/>
+        <bgColor rgb="FF666666"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -66,15 +115,27 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -89,6 +150,10 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -303,39 +368,57 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
+      <c r="B1" s="1"/>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="5">
         <v>1.0</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2">
+    <row r="6">
+      <c r="A6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="5">
         <v>2.0</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2">
+    <row r="7">
+      <c r="A7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="5">
         <v>3.0</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2">
+    <row r="8">
+      <c r="A8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="5">
         <v>1.0</v>
       </c>
     </row>
@@ -355,50 +438,78 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
+      <c r="A1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2">
+      <c r="A2" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="5">
         <v>1.0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2">
+      <c r="A3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="5">
         <v>2.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2">
+      <c r="A4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="5">
         <v>3.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="2">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5">
         <v>3.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2">
+      <c r="A6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="5">
         <v>2.0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
compare normalized names for tube names
</commit_message>
<xml_diff>
--- a/api/tests/acceptance/scripts/target-profile-migrations/migration-test-multiform_1.xlsx
+++ b/api/tests/acceptance/scripts/target-profile-migrations/migration-test-multiform_1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="2005" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="16">
   <si>
     <t xml:space="preserve">Parcours thématique_RGPD &amp; Données personnelles</t>
   </si>
@@ -43,28 +43,31 @@
     <t xml:space="preserve">@codageEmblématique</t>
   </si>
   <si>
+    <t xml:space="preserve">@térmiNal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@editerDocEnLigne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">@partageDroits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coucou</t>
+  </si>
+  <si>
+    <t xml:space="preserve">les</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zamiiiiiiiiiiiiis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id de sujet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">niveau max</t>
+  </si>
+  <si>
     <t xml:space="preserve">@terminal</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@editerDocEnLigne</t>
-  </si>
-  <si>
-    <t xml:space="preserve">@partageDroits</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coucou</t>
-  </si>
-  <si>
-    <t xml:space="preserve">les</t>
-  </si>
-  <si>
-    <t xml:space="preserve">zamiiiiiiiiiiiiis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">id de sujet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">niveau max</t>
   </si>
   <si>
     <t xml:space="preserve">@nimp</t>
@@ -282,11 +285,11 @@
   </sheetPr>
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18"/>
   </cols>
@@ -371,7 +374,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -408,7 +411,7 @@
       <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
@@ -428,7 +431,7 @@
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B3" s="5" t="n">
         <v>2</v>
@@ -452,7 +455,7 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="5" t="n">
         <v>2</v>
@@ -476,11 +479,11 @@
   </sheetPr>
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J22" activeCellId="0" sqref="J22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="64" min="1" style="0" width="12.63"/>
   </cols>
@@ -503,7 +506,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B3" s="5" t="n">
         <v>2</v>
@@ -527,7 +530,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="5" t="n">
         <v>2</v>

</xml_diff>